<commit_message>
Added a new player
</commit_message>
<xml_diff>
--- a/website_data.xlsx
+++ b/website_data.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagarbhargava/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sfl-bidding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD15BA7-0DBB-0641-B5AD-DF5F95941712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E435DF2-A45D-437F-9B33-EE3F72143BB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="500" windowWidth="28800" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="8496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="msfl" sheetId="1" r:id="rId1"/>
     <sheet name="wsfl" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">wsfl!$C$1:$C$34</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -680,14 +683,14 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -709,7 +712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -720,7 +723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -731,7 +734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -742,7 +745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -753,7 +756,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -764,7 +767,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -775,7 +778,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -786,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -797,7 +800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -808,7 +811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -819,7 +822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -830,7 +833,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -841,7 +844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -852,7 +855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -863,7 +866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -874,7 +877,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -885,7 +888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
@@ -896,7 +899,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -907,7 +910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
@@ -918,7 +921,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -929,7 +932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -940,7 +943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -951,7 +954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -962,7 +965,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
@@ -973,7 +976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
@@ -984,7 +987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -995,7 +998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
@@ -1017,7 +1020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
@@ -1083,7 +1086,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>48</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>49</v>
       </c>
@@ -1105,7 +1108,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>50</v>
       </c>
@@ -1116,7 +1119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>51</v>
       </c>
@@ -1127,7 +1130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>52</v>
       </c>
@@ -1138,7 +1141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>54</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>55</v>
       </c>
@@ -1171,7 +1174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>56</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>57</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>58</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>59</v>
       </c>
@@ -1215,7 +1218,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>60</v>
       </c>
@@ -1226,7 +1229,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>61</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>62</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>63</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>64</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>65</v>
       </c>
@@ -1281,7 +1284,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>66</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>67</v>
       </c>
@@ -1303,7 +1306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>68</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>69</v>
       </c>
@@ -1325,7 +1328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>121</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>71</v>
       </c>
@@ -1347,7 +1350,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>72</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>73</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>74</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>75</v>
       </c>
@@ -1391,7 +1394,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>76</v>
       </c>
@@ -1402,7 +1405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>77</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>79</v>
       </c>
@@ -1435,7 +1438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>80</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>81</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>82</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>83</v>
       </c>
@@ -1479,7 +1482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>84</v>
       </c>
@@ -1490,7 +1493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>85</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>86</v>
       </c>
@@ -1512,7 +1515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>87</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>88</v>
       </c>
@@ -1541,21 +1544,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1566,7 +1569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>91</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>92</v>
       </c>
@@ -1599,7 +1602,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>93</v>
       </c>
@@ -1610,7 +1613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>94</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>95</v>
       </c>
@@ -1632,7 +1635,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>96</v>
       </c>
@@ -1643,7 +1646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>97</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>98</v>
       </c>
@@ -1665,7 +1668,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>99</v>
       </c>
@@ -1676,7 +1679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>100</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>101</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>102</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>103</v>
       </c>
@@ -1720,7 +1723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>104</v>
       </c>
@@ -1731,7 +1734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>105</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>106</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>107</v>
       </c>
@@ -1764,7 +1767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>108</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>109</v>
       </c>
@@ -1786,7 +1789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>110</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>111</v>
       </c>
@@ -1808,7 +1811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>112</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>113</v>
       </c>
@@ -1830,7 +1833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>114</v>
       </c>
@@ -1841,7 +1844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>115</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>116</v>
       </c>
@@ -1863,7 +1866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>117</v>
       </c>
@@ -1874,7 +1877,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>118</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>119</v>
       </c>
@@ -1896,7 +1899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>120</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>70</v>
       </c>
@@ -1918,7 +1921,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>122</v>
       </c>
@@ -1930,6 +1933,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C34" xr:uid="{995393D8-D884-40AD-AD04-0A671209A5C5}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Defender"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Defender array updated for MSFL
</commit_message>
<xml_diff>
--- a/website_data.xlsx
+++ b/website_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sfl-bidding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E435DF2-A45D-437F-9B33-EE3F72143BB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E388D38-0DF9-4210-BAC7-A970B1BF9C0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="8496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="8496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="msfl" sheetId="1" r:id="rId1"/>
     <sheet name="wsfl" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">msfl!$A$1:$C$77</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">wsfl!$C$1:$C$34</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -674,13 +675,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -701,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -712,7 +713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -723,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -734,7 +735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -745,7 +746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -756,7 +757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -778,7 +779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -789,7 +790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -800,7 +801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -811,7 +812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -833,7 +834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -855,7 +856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -866,7 +867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -877,7 +878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -899,7 +900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -943,7 +944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -965,7 +966,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
@@ -976,7 +977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
@@ -987,7 +988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -1009,7 +1010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
@@ -1053,7 +1054,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>49</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>52</v>
       </c>
@@ -1141,7 +1142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>54</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>56</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>57</v>
       </c>
@@ -1196,7 +1197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>58</v>
       </c>
@@ -1218,7 +1219,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>60</v>
       </c>
@@ -1229,7 +1230,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>61</v>
       </c>
@@ -1251,7 +1252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>63</v>
       </c>
@@ -1273,7 +1274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>65</v>
       </c>
@@ -1306,7 +1307,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>68</v>
       </c>
@@ -1317,7 +1318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>69</v>
       </c>
@@ -1350,7 +1351,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>72</v>
       </c>
@@ -1361,7 +1362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>73</v>
       </c>
@@ -1372,7 +1373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>74</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>75</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>77</v>
       </c>
@@ -1438,7 +1439,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>80</v>
       </c>
@@ -1449,7 +1450,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>81</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>83</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>85</v>
       </c>
@@ -1515,7 +1516,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>87</v>
       </c>
@@ -1538,6 +1539,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C77" xr:uid="{697884F5-DE2F-41DC-99A2-68240CD553BE}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Defender"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1549,7 +1557,7 @@
   </sheetPr>
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C34"/>
     </sheetView>
   </sheetViews>

</xml_diff>